<commit_message>
Update to Arrays2 questions
</commit_message>
<xml_diff>
--- a/matlab_attempt/Excel problems/Arrays2 questions.xlsx
+++ b/matlab_attempt/Excel problems/Arrays2 questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\QMB-Problem-Maker\matlab_attempt\Excel problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A8015F37-77DA-483F-B318-4B5A2E618961}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E131EAD8-E66B-49E7-A2BD-3B4625073803}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="5" xr2:uid="{36AC9E5E-37B1-4621-9112-0A7D41977D5C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="7" xr2:uid="{36AC9E5E-37B1-4621-9112-0A7D41977D5C}"/>
   </bookViews>
   <sheets>
     <sheet name="CG6.1.1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,10 @@
     <sheet name="CG6.1.4" sheetId="5" r:id="rId4"/>
     <sheet name="CG6.1.5" sheetId="6" r:id="rId5"/>
     <sheet name="CG6.1.6" sheetId="7" r:id="rId6"/>
-    <sheet name="Doesn't work" sheetId="3" r:id="rId7"/>
+    <sheet name="CG6.1.7" sheetId="8" r:id="rId7"/>
+    <sheet name="CG6.2.1" sheetId="9" r:id="rId8"/>
+    <sheet name="Doesn't work" sheetId="3" r:id="rId9"/>
+    <sheet name="Not used" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4047" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4666" uniqueCount="1135">
   <si>
     <t>questionText</t>
   </si>
@@ -3668,6 +3671,496 @@
 &lt;p&gt;
 The other choices are incorrect because they either return the wrong piece or use curly braces instead of parentheses. Curly braces will return the contents of the cells and not the cells themselves.
 &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>struct1</t>
+  </si>
+  <si>
+    <t>STRUCT_NAME</t>
+  </si>
+  <si>
+    <t>randsample({'S','S1','myStruct','myStructure','myStruct1','myS','s','my_struct','my_structure1','my_struct1','s1'},1)</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Given a structure named $STRUCT_NAME/$, write the command that would return the value in a field named $FIELD_NAME/$.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>randsample({'field1','field2','newField','age','height','eyeColor','hairColor','firstName','lastName','name'},1)</t>
+  </si>
+  <si>
+    <t>FIELD_NAME</t>
+  </si>
+  <si>
+    <t>'((\s*\(\s*1\s*\)\s*)|(\s*\(\s*1\s*,\s*1\s*\)\s*))?'</t>
+  </si>
+  <si>
+    <t>ONE</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;
+To access the field in a structure, you use the "dot" notation, e.g. $STRUCT_NAME.FIELD_NAME/$.
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+When referencing a single structure in an array, you need to include an index, e.g. $STRUCT_NAME(1).FIELD_NAME/$. However, this question didn't specify, so $STRUCT_NAME.FIELD_NAME/$ is acceptable. 
+&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>struct2</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Given a structure named $STRUCT_NAME/$, write the command that would store the number $VALUE/$ in a field named $FIELD_NAME/$.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>randsample({'field1','field2','newField','age','height','variable1','mass','var1','field3','val1'},1)</t>
+  </si>
+  <si>
+    <t>'STRUCT_NAMEONE.FIELD_NAMEONE\s*;?'</t>
+  </si>
+  <si>
+    <t>'STRUCT_NAMEONE.FIELD_NAMEONE\s*=\s*VALUE\s*;?'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;
+To store something into a structure field, you use the "dot" notation, e.g. $STRUCT_NAME.FIELD_NAME = VALUE/$.
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+When storing into a single structure in an array, you need to include an index, e.g. $STRUCT_NAME(1).FIELD_NAME = VALUE/$. However, this question didn't specify, so $STRUCT_NAME.FIELD_NAME = VALUE/$ is acceptable. 
+&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>struct3</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Given a structure named $STRUCT_NAME/$, which command would store the number $VALUE/$ in a field named $FIELD_NAME/$.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>[correct,incorrect,problem_values,explanation] = struct3();</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+To store something into a structure field, you use the "dot" notation with a period separating the structure name and the field name. The correct way to store the number $VALUE/$ in a field named $FIELD_NAME/$ is:
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+$$STRUCT_NAME.FIELD_NAME = VALUE/$$
+&lt;/p&gt;
+EXPLAIN</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Given a structure named $STRUCT_NAME/$, which command would return the value in a field named $FIELD_NAME/$.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>struct4</t>
+  </si>
+  <si>
+    <t>[correct,incorrect,problem_values,explanation] = struct4();</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+To return something from a structure field, you use the "dot" notation with a period separating the structure name and the field name. The correct way to return the value in $FIELD_NAME/$ from $STRUCT_NAME/$ is:
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+$$STRUCT_NAME.FIELD_NAME/$$
+&lt;/p&gt;
+EXPLAIN</t>
+  </si>
+  <si>
+    <t>struct5</t>
+  </si>
+  <si>
+    <t>[answer,problem_values,explanation] = struct5();</t>
+  </si>
+  <si>
+    <t>NAME1</t>
+  </si>
+  <si>
+    <t>NAME2</t>
+  </si>
+  <si>
+    <t>NFIELD1</t>
+  </si>
+  <si>
+    <t>NFIELD2</t>
+  </si>
+  <si>
+    <t>SNIPPET</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Consider the following snippet of code.
+&lt;/p&gt;
+&lt;p&gt;
+SNIPPET
+&lt;/p&gt;
+&lt;p&gt;
+How many fields are defined for the structure named $ASK/$?
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+The code snippet creates two structures named $NAME1/$ and $NAME2/$. There are multiple lines that use the "dot" notation to create fields. For example, $NAME1.pet = 'dog'/$ would create a field named $pet/$ with the value $'dog'/$. 
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+The code snippet above defines NFIELD1 fieldADD1 for $NAME1/$ and NFIELD2 fieldADD2 for $NAME2/$. Since this question asks about the structure $ASK/$, the correct answer is $ANS/$.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>ADD1</t>
+  </si>
+  <si>
+    <t>extract({'','s'},(NFIELD2&gt;1)+1)</t>
+  </si>
+  <si>
+    <t>extract({'','s'},(NFIELD1&gt;1)+1)</t>
+  </si>
+  <si>
+    <t>ADD2</t>
+  </si>
+  <si>
+    <t>struct6</t>
+  </si>
+  <si>
+    <t>RANGE</t>
+  </si>
+  <si>
+    <t>MAX_FIELD</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Consider the following snippet of code that creates an array of structures.
+&lt;/p&gt;
+&lt;p&gt;
+SNIPPET
+&lt;/p&gt;
+&lt;p&gt;
+How many structures are created? In other words, what is $length(myStruct)/$.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[4 12] </t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Structures can be placed into arrays just like numbers, characters, or cells. They are indexed in the same way, e.g. $myStruct(2)/$ would reference the 2nd structure in an array named $myStruct/$. A line like $myStruct(3).pet = 'dog'/$ would create a field named $pet/$ with the value $'dog'/$ in the the 3rd structure. The 1st and 2nd structures would have also have the $pet/$ field, but those fields will be empty.  
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+The code snippet above places several fields into different structures of the array $myStruct/$. You can tell the length of $myStruct/$ by looking for the maximum index used in the snippet. In this case, the maximum index is $ANS/$, since a field is assigned for $myStruct(ANS)/$. It does not matter that some indexes are skipped, meaning some structures have no fields assigned. Those structures will still be created, they will simply have all empty fields.
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+Therefore, there are $ANS/$ structures created.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>struct7</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Consider the following snippet of code that creates an array of structures.
+&lt;/p&gt;
+&lt;p&gt;
+SNIPPET
+&lt;/p&gt;
+&lt;p&gt;
+How many fields does $myStruct(IND)/$ have?
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>FRAC_RM</t>
+  </si>
+  <si>
+    <t>[snippet,num_struct] = struct6('array_range',RANGE,'max_fields',MAX_FIELD,'frac_remove',FRAC_RM);</t>
+  </si>
+  <si>
+    <t>num_struct</t>
+  </si>
+  <si>
+    <t>snippet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[4 8] </t>
+  </si>
+  <si>
+    <t>randsample(find(fields_per_struct&gt;0),1)</t>
+  </si>
+  <si>
+    <t>FIELD_STR</t>
+  </si>
+  <si>
+    <t>length(all_fields)</t>
+  </si>
+  <si>
+    <t>[snippet,~,fields_per_struct,all_fields] = struct6('array_range',RANGE,'max_fields',MAX_FIELD,'frac_remove',FRAC_RM);</t>
+  </si>
+  <si>
+    <t>['$' strjoin(all_fields(1:end-1),'/$, $') '/$ and $' all_fields{end} '/$']</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Structures can be placed into arrays just like numbers, characters, or cells. They are indexed in the same way, e.g. $myStruct(2)/$ would reference the 2nd structure in an array named $myStruct/$. A line like $myStruct(3).pet = 'dog'/$ would create a field named $pet/$ with the value $'dog'/$ in the the 3rd structure. The 1st and 2nd structures would have also have the $pet/$ field, but those fields will be empty.  
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+The code snippet above places several fields into different structures of the array $myStruct/$. Any time a field is assigned, that field will be created for every structure in the array; it will simply be empty for non-assigned structures. Therefore, to determine the total number of fields for $myStruct(IND)/$, you need to count the total number of unique fields assigned.
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+In this code snippet, there are $ANS/$ fields assigned: FIELD_STR. The structure $myStruct(IND)/$ will have all these fields, even though some might be empty.  
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+Therefore, $myStruct(IND)/$ has $ANS/$ fields.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>struct8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[2 2] </t>
+  </si>
+  <si>
+    <t>[2 4]</t>
+  </si>
+  <si>
+    <t>struct9</t>
+  </si>
+  <si>
+    <t>NALL</t>
+  </si>
+  <si>
+    <t>fields_per_struct(IND)</t>
+  </si>
+  <si>
+    <t>[2 6]</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Structures can be placed into arrays just like numbers, characters, or cells. They are indexed in the same way, e.g. $myStruct(2)/$ would reference the 2nd structure in an array named $myStruct/$. A line like $myStruct(3).pet = 'dog'/$ would create a field named $pet/$ with the value $'dog'/$ in the the 3rd structure. The 1st and 2nd structures would have also have the $pet/$ field, but those fields will be empty.  
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+The code snippet above places several fields into different structures of the array $myStruct/$. Any time a field is assigned, that field will be created for every structure in the array; it will simply be empty for non-assigned structures. Therefore, to determine the total number of non-empty fields for $myStruct(IND)/$, you need to count the number of lines in which fields assigned to $myStruct(IND)/$.
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+In this code snippet, there are a total of $NALL/$ fields assigned: FIELD_STR. Of these, $ANS/$ fields are assigned to $myStruct(IND)/$. Any other fields will be empty.  
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+Therefore, $myStruct(IND)/$ has $ANS/$ non-empty fields.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Consider the following snippet of code that creates an array of structures.
+&lt;/p&gt;
+&lt;p&gt;
+SNIPPET
+&lt;/p&gt;
+&lt;p&gt;
+How many &lt;em&gt;non-empty&lt;/em&gt; fields does $myStruct(IND)/$ have?
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>struct10</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>VALUES</t>
+  </si>
+  <si>
+    <t>randsample(10,2)</t>
+  </si>
+  <si>
+    <t>extract(VALUES,1)</t>
+  </si>
+  <si>
+    <t>extract(VALUES,2)</t>
+  </si>
+  <si>
+    <t>ARG</t>
+  </si>
+  <si>
+    <t>'STRUCT_NAMEARG.FIELD_NAMEONE\s*;?'</t>
+  </si>
+  <si>
+    <t>'\s*\(\s*IND1\s*,\s*IND2\s*\)\s*'</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Given an array of structures named $STRUCT_NAME/$, write the command that would return the value in a field named $FIELD_NAME/$ from row $IND1/$, column $IND2/$.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>struct11</t>
+  </si>
+  <si>
+    <t>'\s*\(\s*IND1\s*\)\s*'</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Given an array of structures named $STRUCT_NAME/$, write the command that would return the value in a field named $FIELD_NAME/$ from the ORD1 structure in the array (use linear indexing).
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Given an array of structures named $STRUCT_NAME/$, which command would return the value in a field named $FIELD_NAME/$ from the ORD1 structure in the array.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>struct12</t>
+  </si>
+  <si>
+    <t>[correct,incorrect,problem_values,explanation] = struct12();</t>
+  </si>
+  <si>
+    <t>struct13</t>
+  </si>
+  <si>
+    <t>[correct,incorrect,problem_values,explanation] = struct13();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;
+To access a field in a structure, you use the "dot" notation, e.g. $STRUCT_NAME.FIELD_NAME/$. However, since $STRUCT_NAME/$ is an array, you need to index the specific struct in row $IND1/$, column $IND2/$ with the command $STRUCT_NAME(IND1,IND2)/$. Parentheses are used since this is indexing an element in the array, just like accessing a single number from a numeric array. The only difference here is that the element in this case is a structure. Putting these together, the full command is:
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+$$STRUCT_NAME(IND1,IND2).FIELD_NAME/$$
+&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;
+To access a field in a structure, you use the "dot" notation, e.g. $STRUCT_NAME.FIELD_NAME/$. However, since $STRUCT_NAME/$ is an array, you need to index the specific struct in index $IND1/$ with the command $STRUCT_NAME(IND1)/$. Parentheses are used since this is indexing an element in the array, just like accessing a single number from a numeric array. The only difference here is that the element in this case is a structure. Putting these together, the full command is:
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+$$STRUCT_NAME(IND1).FIELD_NAME/$$
+&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+To access a field in a structure, you use the "dot" notation, e.g. $STRUCT_NAME.FIELD_NAME/$. However, since $STRUCT_NAME/$ is an array, you need to index the specific struct in index $IND1/$ with the command $STRUCT_NAME(IND1)/$. Parentheses are used since this is indexing an element in the array, just like accessing a single number from a numeric array. The only difference here is that the element in this case is a structure. Putting these together, the full command is:
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+$$STRUCT_NAME(IND1).FIELD_NAME/$$
+&lt;/p&gt;
+EXPLAIN</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+To access a field in a structure, you use the "dot" notation, e.g. $STRUCT_NAME.FIELD_NAME/$. However, since $STRUCT_NAME/$ is an array, you need to index the specific struct in row $IND1/$, column $IND2/$ with the command $STRUCT_NAME(IND1,IND2)/$. Parentheses are used since this is indexing an element in the array, just like accessing a single number from a numeric array. The only difference here is that the element in this case is a structure. Putting these together, the full command is:
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+$$STRUCT_NAME(IND1,IND2).FIELD_NAME/$$
+&lt;/p&gt;
+EXPLAIN</t>
+  </si>
+  <si>
+    <t>struct14</t>
+  </si>
+  <si>
+    <t>randsample({'randomInteger','randomDouble'},1)</t>
+  </si>
+  <si>
+    <t>randi(30,1)</t>
+  </si>
+  <si>
+    <t>myStruct.CHOICE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;
+Download &lt;a href="/static/randomStructIND.mat" target="_blank"&gt;this file&lt;/a&gt; and load it into Matlab. If you are using Matlab Online, you will need to upload the file before loading it. There should now be a variable named $myStruct/$ in the workspace. $myStruct/$ is a structure with some random data in its fields.
+&lt;/p&gt;
+&lt;p&gt;
+What's the value in the field $CHOICE/$?
+&lt;/p&gt; </t>
+  </si>
+  <si>
+    <t>num2str(ANS)</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+To access a field in a structure, you use the "dot" notation. So to return the data from $myStruct/$ in the field $CHOICE/$, the command is $myStruct.CHOICE/$. You should find that $myStruct.CHOICE/$ has the value $STR/$, so the correct answer is $STR/$.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>load('Data\randomStructIND.mat','myStruct')</t>
+  </si>
+  <si>
+    <t>randsample({'randomString','randomWord'},1)</t>
+  </si>
+  <si>
+    <t>struct15</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+To access a field in a structure, you use the "dot" notation. So to return the data from $myStruct/$ in the field $CHOICE/$, the command is $myStruct.CHOICE/$. You should find that $myStruct.CHOICE/$ has the string $'ANS1'/$, so the correct answer is $'ANS1'/$.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Given an array of structures named $STRUCT_NAME/$, which command would return the value in a field named $FIELD_NAME/$ from row $IND1/$, column $IND2/$.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>struct16</t>
+  </si>
+  <si>
+    <t>STYLE</t>
+  </si>
+  <si>
+    <t>if STYLE==1, field_list = {'field','newField','randomString','randStr','str','myString','myStr'}; end</t>
+  </si>
+  <si>
+    <t>if STYLE==2, struct_list = {'S','my_struct','my_structure','my_array','s','my_data'}; end</t>
+  </si>
+  <si>
+    <t>if STYLE==1, struct_list = {'S','myStruct','myStructure','myArray','s','myData'}; end</t>
+  </si>
+  <si>
+    <t>if STYLE==2, field_list = {'field','new_field','random_string','rand_str','str','my_string','my_str'}; end</t>
+  </si>
+  <si>
+    <t>randsample(struct_list,1)</t>
+  </si>
+  <si>
+    <t>randsample(field_list,1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;
+To store a field in a structure, you use the "dot" notation, e.g. $STRUCT_NAME.FIELD_NAME = 'STRING'/$. However, since $STRUCT_NAME/$ is an array, you need to index the specific struct in row $IND1/$, column $IND2/$ with the command $STRUCT_NAME(IND1,IND2)/$. Parentheses are used since this is indexing an element in the array, just like accessing a single number from a numeric array. The only difference is that the element in this case is a structure. Putting these together, the full command is:
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+$$STRUCT_NAME(IND1,IND2).FIELD_NAME = 'STRING'/$$
+&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>randsample('a':'z',randi([4 5],1))</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Given an array of structures named $STRUCT_NAME/$, write the command that would store the string $'STRING'/$ in a field named $FIELD_NAME/$ into row $IND1/$, column $IND2/$.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>textline</t>
+  </si>
+  <si>
+    <t>'STRUCT_NAMEARG.\s*FIELD_NAME\s*=\s*''STRING''\s*;?'</t>
   </si>
 </sst>
 </file>
@@ -4164,8 +4657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1857D1-1B9B-4FBB-8C88-F9528ED99766}">
   <dimension ref="A1:G475"/>
   <sheetViews>
-    <sheetView topLeftCell="A445" workbookViewId="0">
-      <selection activeCell="C473" sqref="C473"/>
+    <sheetView topLeftCell="A493" workbookViewId="0">
+      <selection activeCell="C454" sqref="C454"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9906,11 +10399,23 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33EC0784-6329-4C34-A626-3BA96DC7D8E2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93A1CCC8-663D-4FFC-B9F4-AFA5CE4136BE}">
   <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A178" workbookViewId="0">
       <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
@@ -11133,7 +11638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F99C37B0-C074-453E-871D-6A511B21862F}">
   <dimension ref="A1:F255"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A292" workbookViewId="0">
       <selection activeCell="B35" sqref="B35:C39"/>
     </sheetView>
   </sheetViews>
@@ -14046,7 +14551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3809CDA-EBD7-4FFA-9CAD-F80442A2CEED}">
   <dimension ref="A1:E162"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A148" workbookViewId="0">
       <selection activeCell="D159" sqref="D159"/>
     </sheetView>
   </sheetViews>
@@ -15790,8 +16295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D99631B9-D9E9-4E65-BEFA-286507439774}">
   <dimension ref="A1:E221"/>
   <sheetViews>
-    <sheetView topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="C201" sqref="C201"/>
+    <sheetView topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="B170" sqref="A170:XFD172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18243,8 +18748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03573DE7-FA0C-474B-B66E-2AD9A3986D0A}">
   <dimension ref="A1:F249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="E239" sqref="E239"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21022,11 +21527,2628 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ABC6F1-B53A-4F71-800C-85B0A26FEF72}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE8B832-9851-4C4F-9DE7-5E000953A1D7}">
+  <dimension ref="A1:E247"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="C235" sqref="C235"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E6" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="B7" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>924</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>1087</v>
+      </c>
+      <c r="E18" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="B19" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>924</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>1087</v>
+      </c>
+      <c r="E36" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E40" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="B41" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B51" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B52" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B53" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B54" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E54" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B55" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E55" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B56" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E56" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B57" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E57" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B58" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E58" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="B59" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B60" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C61" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B63" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B64" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B65" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B66" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B67" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B68" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B69" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B70" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B71" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B72" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B73" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>1087</v>
+      </c>
+      <c r="E73" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="B74" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B75" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B76" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C76" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C77" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B79" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B80" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D80" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B81" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D81" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B82" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B83" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B84" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B85" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E85" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="280.5" x14ac:dyDescent="0.2">
+      <c r="B86" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B87" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B88" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C88" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C89" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C90" s="12" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B91" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C91" s="12" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B92" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D92" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B93" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C93" s="12" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D93" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B94" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B95" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B96" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B97" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B98" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B99" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E99" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="318.75" x14ac:dyDescent="0.2">
+      <c r="B100" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B101" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B102" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C102" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C103" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" s="12" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B105" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C105" s="12" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B106" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C106" s="12" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B107" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D107" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B108" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B109" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B110" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B111" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B112" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B113" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E113" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="318.75" x14ac:dyDescent="0.2">
+      <c r="B114" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B115" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B116" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C116" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C117" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A118" s="4" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C118" s="12" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B119" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C119" s="12" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B120" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C120" s="12" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B121" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C121" s="12" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D121" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B122" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B123" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B124" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B125" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B126" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B127" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B128" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E128" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="331.5" x14ac:dyDescent="0.2">
+      <c r="B129" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B130" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B131" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C131" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B132" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C132" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B134" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B135" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B136" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B137" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B138" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D138" s="4" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B139" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D139" s="18" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B140" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D140" s="18" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B141" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D141" s="18" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B142" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E142" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="B143" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C143" s="21" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B144" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B145" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C145" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B146" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C146" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B147" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C147" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B149" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B150" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D150" s="4" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B151" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D151" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B152" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C152" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D152" s="4" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B153" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D153" s="18" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B154" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C154" s="4" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D154" s="18" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B155" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C155" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D155" s="18" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B156" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C156" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D156" s="4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E156" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="B157" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C157" s="21" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B158" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B159" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C159" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B160" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C160" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B161" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C161" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A162" s="1" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B163" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C163" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D163" s="4" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B164" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C164" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D164" s="4" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B165" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C165" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D165" s="4" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B166" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C166" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D166" s="19" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B167" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C167" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D167" s="19" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B168" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C168" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D168" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B169" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D169" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B170" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C170" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D170" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B171" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C171" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D171" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B172" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C172" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D172" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B173" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C173" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D173" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B174" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D174" s="4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E174" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B175" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C175" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E175" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B176" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C176" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E176" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B177" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C177" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E177" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B178" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C178" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E178" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="B179" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C179" s="21" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B180" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C180" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B181" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C181" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A182" s="4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B182" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B183" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C183" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D183" s="4" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B184" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C184" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D184" s="4" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B185" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C185" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D185" s="4" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" s="19"/>
+      <c r="B186" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C186" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D186" s="19" t="s">
+        <v>715</v>
+      </c>
+      <c r="E186" s="19"/>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187" s="19"/>
+      <c r="B187" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C187" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D187" s="19" t="s">
+        <v>716</v>
+      </c>
+      <c r="E187" s="19"/>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188" s="19"/>
+      <c r="B188" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C188" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D188" s="19" t="s">
+        <v>750</v>
+      </c>
+      <c r="E188" s="19"/>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189" s="19"/>
+      <c r="B189" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C189" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D189" s="19" t="s">
+        <v>800</v>
+      </c>
+      <c r="E189" s="19"/>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B190" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C190" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D190" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B191" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C191" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D191" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B192" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C192" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D192" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B193" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C193" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D193" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B194" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C194" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D194" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B195" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C195" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D195" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B196" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C196" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E196" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B197" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C197" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E197" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B198" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C198" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E198" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B199" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C199" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E199" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B200" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C200" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E200" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="B201" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C201" s="21" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B202" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C202" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B203" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C203" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A204" s="4" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C204" s="12" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B205" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C205" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D205" s="4" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B206" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C206" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D206" s="4" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B207" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C207" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D207" s="4" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B208" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C208" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D208" s="4" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B209" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C209" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D209" s="4" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B210" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C210" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D210" s="4" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E210" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B211" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C211" s="21" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B212" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B213" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C213" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B214" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C214" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A215" s="4" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B215" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C215" s="12" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B216" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C216" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D216" s="4" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B217" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C217" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D217" s="4" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B218" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C218" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D218" s="4" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B219" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C219" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D219" s="4" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B220" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C220" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D220" s="18" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B221" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C221" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D221" s="4" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E221" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B222" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C222" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D222" s="4" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E222" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B223" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C223" s="21" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B224" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B225" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C225" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B226" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C226" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A227" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228" s="1"/>
+      <c r="B228" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D228" s="4" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229" s="1"/>
+      <c r="B229" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D229" s="4" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230" s="1"/>
+      <c r="B230" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D230" s="4" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231" s="1"/>
+      <c r="B231" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D231" s="4" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232" s="1"/>
+      <c r="B232" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D232" s="4" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B233" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C233" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D233" s="4" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B234" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C234" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D234" s="4" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B235" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C235" s="4" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D235" s="4" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B236" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C236" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D236" s="4" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B237" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C237" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D237" s="4" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B238" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C238" s="4" t="s">
+        <v>946</v>
+      </c>
+      <c r="D238" s="4" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B239" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C239" s="4" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D239" s="18" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B240" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C240" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D240" s="18" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="241" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B241" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C241" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D241" s="4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E241" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="2:5" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="B242" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C242" s="21" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="243" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B243" s="13" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C243" s="21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="244" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B244" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C244" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="245" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B245" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C245" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B246" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C246" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B247" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C247" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1D4546-A249-41C9-8A27-1F475BBFF37B}">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="A1:E25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added some struct questions and KCs
</commit_message>
<xml_diff>
--- a/matlab_attempt/Excel problems/Arrays2 questions.xlsx
+++ b/matlab_attempt/Excel problems/Arrays2 questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\QMB-Problem-Maker\matlab_attempt\Excel problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E131EAD8-E66B-49E7-A2BD-3B4625073803}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7393E82F-0CA4-410C-A641-3CBD172389DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="7" xr2:uid="{36AC9E5E-37B1-4621-9112-0A7D41977D5C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4666" uniqueCount="1135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4904" uniqueCount="1186">
   <si>
     <t>questionText</t>
   </si>
@@ -4161,6 +4161,223 @@
   </si>
   <si>
     <t>'STRUCT_NAMEARG.\s*FIELD_NAME\s*=\s*''STRING''\s*;?'</t>
+  </si>
+  <si>
+    <t>struct17</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Consider the following snippet of code that creates an array of structures.
+&lt;/p&gt;
+&lt;p&gt;
+SNIPPET
+&lt;/p&gt;
+&lt;p&gt;
+What is $length([STRUCT_NAME.FIELD_NAME])/$?
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>output{1}</t>
+  </si>
+  <si>
+    <t>output{2}</t>
+  </si>
+  <si>
+    <t>output{3}</t>
+  </si>
+  <si>
+    <t>output{4}</t>
+  </si>
+  <si>
+    <t>output{5}</t>
+  </si>
+  <si>
+    <t>length(INDEXES)</t>
+  </si>
+  <si>
+    <t>EMPTY</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Since $STRUCT_NAME/$ is an array, the command $STRUCT_NAME.FIELD_NAME/$ will iteratively output each value assigned to a $FIELD_NAME/$ field. Adding square brackets will join these values together in an array, so $[STRUCT_NAME.FIELD_NAME]/$ will be an array of integers with each value of $FIELD_NAME/$. 
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+This snippet of code does not assign a value of $FIELD_NAME/$ for each structure in the array. For example, $STRUCT_NAME(EMPTY).FIELD_NAME/$ is not assigned, so it will be an empty array $[]/$. When Matlab joins together all the values of $FIELD_NAME/$ into an array, these empty arrays do not add anything to the final length of the array. For example, the output of $[0, 0, [], 0]/$ is 1x3 array of zeros.
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+Therefore, only the assigned values of $FIELD_NAME/$ will be in the array $[STRUCT_NAME.FIELD_NAME]/$. There are $ANS/$ values assigned in to $FIELD_NAME/$, so the length of $[STRUCT_NAME.FIELD_NAME]/$ is $ANS/$.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>output = struct17('max_lines',15,'range_lines',[4 10],'max_value',100);</t>
+  </si>
+  <si>
+    <t>struct18</t>
+  </si>
+  <si>
+    <t>extract(VALUES,IND)</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Consider the following snippet of code that creates an array of structures.
+&lt;/p&gt;
+&lt;p&gt;
+SNIPPET
+&lt;/p&gt;
+&lt;p&gt;
+If you now set $x = [STRUCT_NAME.FIELD_NAME]/$, what is $x(IND)/$?
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>ARRAY</t>
+  </si>
+  <si>
+    <t>mat2string(VALUES)</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Since $STRUCT_NAME/$ is an array of structures, the command $STRUCT_NAME.FIELD_NAME/$ will iteratively output each value assigned to a $FIELD_NAME/$ field. Adding square brackets will join these values together in an array, so $x = [STRUCT_NAME.FIELD_NAME]/$ will create an array named $x/$ that has the all the integers in $FIELD_NAME/$ fields. 
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+This snippet of code does not assign a value of $FIELD_NAME/$ for each structure in the array. For example, $STRUCT_NAME(EMPTY).FIELD_NAME/$ is not assigned, so it will be an empty array $[]/$. When Matlab joins together all the values of $FIELD_NAME/$ into an array, these empty arrays do not add anything to the final length of the array. For example, the output of $[0, 0, [], 0]/$ is 1x3 array of zeros.
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+In other words, the line $x = [STRUCT_NAME.FIELD_NAME]/$ will only assign the filled values of $FIELD_NAME/$ into $x/$, i.e. the values $ARRAY/$. The statement $x(IND)/$ will return the ORD value in this array: $ANS/$. Therefore, the answer is $ANS/$.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Consider the following snippet of code that creates an array of structures.
+&lt;/p&gt;
+&lt;p&gt;
+SNIPPET
+&lt;/p&gt;
+&lt;p&gt;
+What is $length({STRUCT_NAME.FIELD_NAME})/$?
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>struct19</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Since $STRUCT_NAME/$ is an array, the command $STRUCT_NAME.FIELD_NAME/$ will iteratively output each string assigned to a $FIELD_NAME/$ field. Adding curly braces will join these values together in a cell array, so ${STRUCT_NAME.FIELD_NAME}/$ will be a cell array of strings that has each value of $FIELD_NAME/$. 
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+This snippet of code does not assign a string to $FIELD_NAME/$ for each structure in the array. For example, $STRUCT_NAME(EMPTY).FIELD_NAME/$ is not assigned, so it will be an empty array $[]/$. When Matlab joins together all the values of $FIELD_NAME/$ into an array, these empty arrays &lt;em&gt;do&lt;/em&gt; contribute to the final length of the array. For example, the output of ${'hello', -4.2, [], 'bye'}/$ is 1x4 cell array with an empty array in the 3rd cell.
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+Therefore, both the filled and empty values of $FIELD_NAME/$ will be in the array ${STRUCT_NAME.FIELD_NAME}/$. The array $STRUCT_NAME/$ has a length of $ANS/$  because a string is assigned to $STRUCT_NAME(ANS)/$, so the length of ${STRUCT_NAME.FIELD_NAME}/$ is $ANS/$.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>MAX_LINES</t>
+  </si>
+  <si>
+    <t>randi([10 15],1)</t>
+  </si>
+  <si>
+    <t>output = struct17('max_lines',MAX_LINES,'range_lines',[3 8],'do_words',true);</t>
+  </si>
+  <si>
+    <t>max(INDEXES)</t>
+  </si>
+  <si>
+    <t>struct20</t>
+  </si>
+  <si>
+    <t>'The string $''STRING1''/$'</t>
+  </si>
+  <si>
+    <t>'An empty array $[]/$'</t>
+  </si>
+  <si>
+    <t>'The string $''STRING2''/$'</t>
+  </si>
+  <si>
+    <t>EMPTY_IND</t>
+  </si>
+  <si>
+    <t>FILLED_IND1</t>
+  </si>
+  <si>
+    <t>IS_EMPTY</t>
+  </si>
+  <si>
+    <t>rand&lt;0.333</t>
+  </si>
+  <si>
+    <t>ask_ind</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Consider the following snippet of code that creates an array of structures.
+&lt;/p&gt;
+&lt;p&gt;
+SNIPPET
+&lt;/p&gt;
+&lt;p&gt;
+If you now set $x = {STRUCT_NAME.FIELD_NAME}/$, what is $x{ASK_IND}/$?
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>find(~ismember(1:max(INDEXES),INDEXES),1)</t>
+  </si>
+  <si>
+    <t>extract(INDEXES,filled_inds(1))</t>
+  </si>
+  <si>
+    <t>output{5}{filled_inds(1)}</t>
+  </si>
+  <si>
+    <t>output{5}{filled_inds(2)}</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Since $STRUCT_NAME/$ is an array, the command $STRUCT_NAME.FIELD_NAME/$ will iteratively output each string assigned to a $FIELD_NAME/$ field. Adding curly braces will join these values together in a cell array, so $x/$ will be a cell array of strings that has each value of $FIELD_NAME/$. 
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+This snippet of code does not assign a string to $FIELD_NAME/$ for each structure in the array. For example, $STRUCT_NAME(EMPTY_IND).FIELD_NAME/$ is not assigned, so it will be an empty array $[]/$. When Matlab joins together all the values of $FIELD_NAME/$ into a cell array, these empty arrays will be placed into cells. The variable $x/$ will be a 1xLEN cell array containing both strings and empty arrays.
+&lt;/p&gt;&lt;br/&gt;
+&lt;p&gt;
+The value stored in $x{ASK_IND}/$ is the same as $STRUCT_NAME(ASK_IND).FIELD_NAME/$. EXPLAIN
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>if IS_EMPTY, explain = 'This is an empty array because a string was not assigned to this field. Therefore, the correct answer is "An empty array $[]/$".'; end</t>
+  </si>
+  <si>
+    <t>randsample(find(~ismember(1:LEN,INDEXES)),1)</t>
+  </si>
+  <si>
+    <t>if ~IS_EMPTY, explain = 'This is the string $''STRING1''/$. Therefore, the correct answer is "The string $''STRING1''/$".'; end</t>
+  </si>
+  <si>
+    <t>'The string $''STRING3''/$'</t>
+  </si>
+  <si>
+    <t>if ~IS_EMPTY, ask_ind = FILLED_IND1; is_correct = convert_logical([1 0 0 0 0]); end</t>
+  </si>
+  <si>
+    <t>if IS_EMPTY, ask_ind = EMPTY_IND; is_correct = convert_logical([0 0 0 1 0]); end</t>
+  </si>
+  <si>
+    <t>output{5}{filled_inds(3)}</t>
+  </si>
+  <si>
+    <t>randi([13 15],1)</t>
+  </si>
+  <si>
+    <t>filled_inds = randsample(1:length(INDEXES),3);</t>
+  </si>
+  <si>
+    <t>C14, C15, C1, C3</t>
+  </si>
+  <si>
+    <t>C14, C15, C3</t>
+  </si>
+  <si>
+    <t>C14, C15</t>
   </si>
 </sst>
 </file>
@@ -4657,7 +4874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1857D1-1B9B-4FBB-8C88-F9528ED99766}">
   <dimension ref="A1:G475"/>
   <sheetViews>
-    <sheetView topLeftCell="A493" workbookViewId="0">
+    <sheetView topLeftCell="A418" workbookViewId="0">
       <selection activeCell="C454" sqref="C454"/>
     </sheetView>
   </sheetViews>
@@ -11638,7 +11855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F99C37B0-C074-453E-871D-6A511B21862F}">
   <dimension ref="A1:F255"/>
   <sheetViews>
-    <sheetView topLeftCell="A292" workbookViewId="0">
+    <sheetView topLeftCell="A211" workbookViewId="0">
       <selection activeCell="B35" sqref="B35:C39"/>
     </sheetView>
   </sheetViews>
@@ -16295,8 +16512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D99631B9-D9E9-4E65-BEFA-286507439774}">
   <dimension ref="A1:E221"/>
   <sheetViews>
-    <sheetView topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="B170" sqref="A170:XFD172"/>
+    <sheetView topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="B195" sqref="A195:XFD199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18748,7 +18965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03573DE7-FA0C-474B-B66E-2AD9A3986D0A}">
   <dimension ref="A1:F249"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A238" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:C10"/>
     </sheetView>
   </sheetViews>
@@ -21540,10 +21757,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE8B832-9851-4C4F-9DE7-5E000953A1D7}">
-  <dimension ref="A1:E247"/>
+  <dimension ref="A1:E332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="C235" sqref="C235"/>
+    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="C242" sqref="C242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21551,7 +21768,9 @@
     <col min="1" max="1" width="11.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="4"/>
+    <col min="4" max="4" width="20.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -24075,7 +24294,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="241" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B241" s="4" t="s">
         <v>40</v>
       </c>
@@ -24089,7 +24308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="2:5" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:5" ht="178.5" x14ac:dyDescent="0.2">
       <c r="B242" s="13" t="s">
         <v>45</v>
       </c>
@@ -24097,7 +24316,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="243" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B243" s="13" t="s">
         <v>1133</v>
       </c>
@@ -24105,7 +24324,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="244" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B244" s="16" t="s">
         <v>42</v>
       </c>
@@ -24113,7 +24332,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="245" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B245" s="16" t="s">
         <v>110</v>
       </c>
@@ -24121,7 +24340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B246" s="16" t="s">
         <v>111</v>
       </c>
@@ -24129,11 +24348,925 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B247" s="17" t="s">
         <v>44</v>
       </c>
       <c r="C247" s="17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A248" s="4" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B248" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C248" s="12" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B249" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C249" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D249" s="4" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B250" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C250" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D250" s="4" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B251" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C251" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D251" s="4" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B252" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C252" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D252" s="4" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B253" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C253" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="D253" s="4" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B254" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C254" s="4" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D254" s="4" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B255" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C255" s="4" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D255" s="4" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B256" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C256" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D256" s="4" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B257" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C257" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D257" s="4" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E257" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" ht="280.5" x14ac:dyDescent="0.2">
+      <c r="B258" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C258" s="21" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B259" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B260" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C260" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B261" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C261" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A262" s="4" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B262" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C262" s="12" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B263" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C263" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D263" s="4" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B264" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C264" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D264" s="4" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B265" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C265" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D265" s="4" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B266" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C266" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D266" s="4" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B267" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C267" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="D267" s="4" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B268" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C268" s="4" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D268" s="4" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B269" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C269" s="4" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D269" s="4" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B270" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C270" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D270" s="4" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B271" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C271" s="4" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D271" s="4" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B272" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C272" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D272" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B273" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C273" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D273" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B274" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C274" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D274" s="4" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B275" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C275" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D275" s="4" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E275" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" ht="293.25" x14ac:dyDescent="0.2">
+      <c r="B276" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C276" s="21" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B277" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B278" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C278" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B279" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C279" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A280" s="4" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B280" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C280" s="12" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B281" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C281" s="12" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D281" s="4" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B282" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C282" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D282" s="4" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B283" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C283" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D283" s="4" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B284" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C284" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D284" s="4" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B285" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C285" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D285" s="4" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B286" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C286" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="D286" s="4" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B287" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C287" s="4" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D287" s="4" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B288" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C288" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D288" s="4" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B289" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C289" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D289" s="18" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E289" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" ht="318.75" x14ac:dyDescent="0.2">
+      <c r="B290" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C290" s="21" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B291" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B292" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C292" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B293" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C293" s="28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A294" s="4" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B294" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C294" s="12" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B295" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C295" s="12" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D295" s="4" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B296" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C296" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D296" s="4" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B297" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C297" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D297" s="4" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B298" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C298" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D298" s="4" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B299" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C299" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D299" s="4" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B300" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C300" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="D300" s="4" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B301" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C301" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D301" s="4" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B302" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C302" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D302" s="4" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B303" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C303" s="4" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D303" s="4" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B304" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C304" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D304" s="4" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="305" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B305" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C305" s="4" t="s">
+        <v>829</v>
+      </c>
+      <c r="D305" s="4" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="306" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B306" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C306" s="4" t="s">
+        <v>870</v>
+      </c>
+      <c r="D306" s="4" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="307" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B307" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C307" s="4" t="s">
+        <v>1163</v>
+      </c>
+      <c r="D307" s="4" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="308" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B308" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C308" s="4" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D308" s="4" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="309" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B309" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C309" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D309" s="4" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="310" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B310" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C310" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D310" s="4" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="311" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B311" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C311" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="D311" s="4" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="312" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B312" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C312" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="D312" s="4" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="313" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B313" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C313" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="D313" s="4" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="314" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B314" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C314" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="D314" s="4" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="315" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B315" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C315" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D315" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="316" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B316" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C316" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="D316" s="4" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="317" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B317" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C317" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D317" s="18" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="318" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B318" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C318" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D318" s="18" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="319" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B319" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C319" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D319" s="18" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="320" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B320" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C320" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D320" s="18" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="321" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B321" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C321" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D321" s="18" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="322" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B322" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C322" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D322" s="18" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="323" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B323" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C323" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D323" s="18" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="324" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B324" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C324" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D324" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="325" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B325" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C325" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D325" s="18" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E325" s="4" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="326" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B326" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C326" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D326" s="18" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E326" s="4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="327" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B327" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C327" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D327" s="18" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E327" s="4" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="328" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B328" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C328" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D328" s="18" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E328" s="4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="329" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B329" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C329" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D329" s="18" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E329" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="330" spans="2:5" ht="255" x14ac:dyDescent="0.2">
+      <c r="B330" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C330" s="21" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="331" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B331" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="332" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B332" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C332" s="28" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update for Mar 6 version of problems
</commit_message>
<xml_diff>
--- a/matlab_attempt/Excel problems/Arrays2 questions.xlsx
+++ b/matlab_attempt/Excel problems/Arrays2 questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\QMB-Problem-Maker\matlab_attempt\Excel problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EE6A54-F396-48F0-B51D-6A4E54CD12D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65DF845-40DB-446C-84C3-EC2A4BEB9112}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{36AC9E5E-37B1-4621-9112-0A7D41977D5C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="6" xr2:uid="{36AC9E5E-37B1-4621-9112-0A7D41977D5C}"/>
   </bookViews>
   <sheets>
     <sheet name="CG6.1.1" sheetId="1" r:id="rId1"/>
@@ -5166,8 +5166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1857D1-1B9B-4FBB-8C88-F9528ED99766}">
   <dimension ref="A1:G476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A289" workbookViewId="0">
-      <selection activeCell="C293" sqref="C293"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22116,7 +22116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE8B832-9851-4C4F-9DE7-5E000953A1D7}">
   <dimension ref="A1:E475"/>
   <sheetViews>
-    <sheetView topLeftCell="A186" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
       <selection activeCell="B372" sqref="B372"/>
     </sheetView>
   </sheetViews>

</xml_diff>